<commit_message>
add tool and dsl implementation
</commit_message>
<xml_diff>
--- a/xModels&Tests/XPSSM-data/PSSM.Overall.xlsx
+++ b/xModels&Tests/XPSSM-data/PSSM.Overall.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\labtop\GitHub\xtdl_FaultLocalization\org.imt.tdl.sbfl.evaluation\evaluationData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\labtop\gemoc_studio\workspaces\xTDL_FaultLocalization\runtime-coverage\XPSSM-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B817318-6B6C-4EAB-8A17-3319AB20DC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EBD67E-4D91-47A5-8B4C-AF65AB365F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JavaEJB" sheetId="1" r:id="rId1"/>
     <sheet name="BankATM" sheetId="2" r:id="rId2"/>
-    <sheet name="Average " sheetId="3" r:id="rId3"/>
+    <sheet name="JavaThread" sheetId="4" r:id="rId3"/>
+    <sheet name="OnlineShopping" sheetId="5" r:id="rId4"/>
+    <sheet name="Average " sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="34">
   <si>
     <t>SBFL Technique</t>
   </si>
@@ -133,6 +135,12 @@
   <si>
     <t>BankATM</t>
   </si>
+  <si>
+    <t>JavaThread</t>
+  </si>
+  <si>
+    <t>OnlineShopping</t>
+  </si>
 </sst>
 </file>
 
@@ -200,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -293,11 +301,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -306,53 +323,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1944,332 +1958,1764 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{997BA24F-2B09-47FE-954C-79BDA0805054}">
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="C2">
+        <v>0.216</v>
+      </c>
+      <c r="D2">
+        <v>0.215</v>
+      </c>
+      <c r="E2">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="F2">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="G2">
+        <v>0.31</v>
+      </c>
+      <c r="H2">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="I2">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="J2">
+        <v>0.44700000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0.114</v>
+      </c>
+      <c r="C3">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="D3">
+        <v>0.255</v>
+      </c>
+      <c r="E3">
+        <v>0.224</v>
+      </c>
+      <c r="F3">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="G3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H3">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="I3">
+        <v>0.375</v>
+      </c>
+      <c r="J3">
+        <v>0.35299999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="C4">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="D4">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="E4">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="F4">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="G4">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H4">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="I4">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="J4">
+        <v>0.33800000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="C5">
+        <v>0.223</v>
+      </c>
+      <c r="D5">
+        <v>0.215</v>
+      </c>
+      <c r="E5">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="G5">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="H5">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="I5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J5">
+        <v>0.441</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="C6">
+        <v>0.214</v>
+      </c>
+      <c r="D6">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="E6">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="G6">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="H6">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="I6">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="J6">
+        <v>0.43099999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C7">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="D7">
+        <v>0.224</v>
+      </c>
+      <c r="E7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="G7">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="H7">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="I7">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="J7">
+        <v>0.34899999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C8">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="D8">
+        <v>0.224</v>
+      </c>
+      <c r="E8">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="G8">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="H8">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="I8">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="J8">
+        <v>0.34899999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="C9">
+        <v>0.222</v>
+      </c>
+      <c r="D9">
+        <v>0.214</v>
+      </c>
+      <c r="E9">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="F9">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="G9">
+        <v>0.307</v>
+      </c>
+      <c r="H9">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="I9">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="J9">
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="C10">
+        <v>0.25</v>
+      </c>
+      <c r="D10">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="E10">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="F10">
+        <v>0.315</v>
+      </c>
+      <c r="G10">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="H10">
+        <v>0.309</v>
+      </c>
+      <c r="I10">
+        <v>0.38</v>
+      </c>
+      <c r="J10">
+        <v>0.34599999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>0.114</v>
+      </c>
+      <c r="C11">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="D11">
+        <v>0.255</v>
+      </c>
+      <c r="E11">
+        <v>0.224</v>
+      </c>
+      <c r="F11">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="G11">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="H11">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="I11">
+        <v>0.376</v>
+      </c>
+      <c r="J11">
+        <v>0.35199999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="C12">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.217</v>
+      </c>
+      <c r="E12">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="F12">
+        <v>0.4</v>
+      </c>
+      <c r="G12">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="H12">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="I12">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="J12">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="C13">
+        <v>0.221</v>
+      </c>
+      <c r="D13">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="E13">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="F13">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="G13">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="H13">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="I13">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J13">
+        <v>0.441</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="C14">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D14">
+        <v>0.19</v>
+      </c>
+      <c r="E14">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="F14">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="G14">
+        <v>0.251</v>
+      </c>
+      <c r="H14">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="I14">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="J14">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="C15">
+        <v>0.222</v>
+      </c>
+      <c r="D15">
+        <v>0.214</v>
+      </c>
+      <c r="E15">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="F15">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="G15">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="H15">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="I15">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J15">
+        <v>0.441</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="C16">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="D16">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="E16">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="F16">
+        <v>0.443</v>
+      </c>
+      <c r="G16">
+        <v>0.251</v>
+      </c>
+      <c r="H16">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="I16">
+        <v>0.65</v>
+      </c>
+      <c r="J16">
+        <v>0.35099999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D17">
+        <v>2E-3</v>
+      </c>
+      <c r="E17">
+        <v>0.5</v>
+      </c>
+      <c r="F17">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="G17">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="H17">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="I17">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="J17">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>0.114</v>
+      </c>
+      <c r="C18">
+        <v>0.152</v>
+      </c>
+      <c r="D18">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="E18">
+        <v>0.5</v>
+      </c>
+      <c r="F18">
+        <v>0.35</v>
+      </c>
+      <c r="G18">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="H18">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="I18">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="J18">
+        <v>0.45700000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="C19">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="D19">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="E19">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="F19">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="G19">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="H19">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="I19">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="J19">
+        <v>0.307</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C20">
+        <v>0.153</v>
+      </c>
+      <c r="D20">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="E20">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F20">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="G20">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="H20">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="I20">
+        <v>0.39</v>
+      </c>
+      <c r="J20">
+        <v>0.40300000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9659806-4728-4418-A2C3-A3D2731E1DBC}">
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C2">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="D2">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="E2">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="F2">
+        <v>0.439</v>
+      </c>
+      <c r="G2">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="H2">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="I2">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="J2">
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C3">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="E3">
+        <v>0.34</v>
+      </c>
+      <c r="F3">
+        <v>0.318</v>
+      </c>
+      <c r="G3">
+        <v>0.253</v>
+      </c>
+      <c r="H3">
+        <v>0.505</v>
+      </c>
+      <c r="I3">
+        <v>0.46</v>
+      </c>
+      <c r="J3">
+        <v>0.32600000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="C4">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="D4">
+        <v>0.377</v>
+      </c>
+      <c r="E4">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="F4">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="G4">
+        <v>0.34</v>
+      </c>
+      <c r="H4">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="I4">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="J4">
+        <v>0.32800000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>0.216</v>
+      </c>
+      <c r="C5">
+        <v>0.248</v>
+      </c>
+      <c r="D5">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="E5">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="F5">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="G5">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="H5">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="I5">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="J5">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C6">
+        <v>0.222</v>
+      </c>
+      <c r="D6">
+        <v>0.214</v>
+      </c>
+      <c r="E6">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="F6">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="G6">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="H6">
+        <v>0.99</v>
+      </c>
+      <c r="I6">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="J6">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C7">
+        <v>0.112</v>
+      </c>
+      <c r="D7">
+        <v>0.17</v>
+      </c>
+      <c r="E7">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="G7">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="H7">
+        <v>0.124</v>
+      </c>
+      <c r="I7">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="J7">
+        <v>0.32300000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C8">
+        <v>0.112</v>
+      </c>
+      <c r="D8">
+        <v>0.17</v>
+      </c>
+      <c r="E8">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="G8">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="H8">
+        <v>0.124</v>
+      </c>
+      <c r="I8">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="J8">
+        <v>0.32300000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>0.185</v>
+      </c>
+      <c r="C9">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.21</v>
+      </c>
+      <c r="E9">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="F9">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="G9">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="H9">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="I9">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="J9">
+        <v>0.41899999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="D10">
+        <v>0.218</v>
+      </c>
+      <c r="E10">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="F10">
+        <v>0.37</v>
+      </c>
+      <c r="G10">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="H10">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="I10">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="J10">
+        <v>0.29899999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C11">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="D11">
+        <v>0.23</v>
+      </c>
+      <c r="E11">
+        <v>0.34</v>
+      </c>
+      <c r="F11">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="G11">
+        <v>0.252</v>
+      </c>
+      <c r="H11">
+        <v>0.505</v>
+      </c>
+      <c r="I11">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="J11">
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>0.216</v>
+      </c>
+      <c r="C12">
+        <v>0.248</v>
+      </c>
+      <c r="D12">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="E12">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="F12">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="G12">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="H12">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="I12">
+        <v>0.66</v>
+      </c>
+      <c r="J12">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C13">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="D13">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="E13">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="F13">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="G13">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="H13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="I13">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="J13">
+        <v>0.41299999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>0.216</v>
+      </c>
+      <c r="C14">
+        <v>0.247</v>
+      </c>
+      <c r="D14">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="E14">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="F14">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="G14">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="H14">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="I14">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="J14">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="C15">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D15">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="E15">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="F15">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="G15">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="H15">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="I15">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="J15">
+        <v>0.40699999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="C16">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="D16">
+        <v>0.187</v>
+      </c>
+      <c r="E16">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="F16">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="G16">
+        <v>0.224</v>
+      </c>
+      <c r="H16">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="I16">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="J16">
+        <v>0.32200000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>0.01</v>
+      </c>
+      <c r="C17">
+        <v>0.01</v>
+      </c>
+      <c r="D17">
+        <v>1E-3</v>
+      </c>
+      <c r="E17">
+        <v>0.5</v>
+      </c>
+      <c r="F17">
+        <v>0.5</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0.99</v>
+      </c>
+      <c r="I17">
+        <v>0.99</v>
+      </c>
+      <c r="J17">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>6.2E-2</v>
+      </c>
+      <c r="C18">
+        <v>0.129</v>
+      </c>
+      <c r="D18">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="E18">
+        <v>0.5</v>
+      </c>
+      <c r="F18">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="G18">
+        <v>0.255</v>
+      </c>
+      <c r="H18">
+        <v>0.99</v>
+      </c>
+      <c r="I18">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="J18">
+        <v>0.42799999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>0.495</v>
+      </c>
+      <c r="C19">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="D19">
+        <v>0.217</v>
+      </c>
+      <c r="E19">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="F19">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="G19">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="H19">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="I19">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="J19">
+        <v>0.28399999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>0.01</v>
+      </c>
+      <c r="C20">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="D20">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="E20">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F20">
+        <v>0.218</v>
+      </c>
+      <c r="G20">
+        <v>0.249</v>
+      </c>
+      <c r="H20">
+        <v>0.124</v>
+      </c>
+      <c r="I20">
+        <v>0.34</v>
+      </c>
+      <c r="J20">
+        <v>0.374</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44F4AD7-7617-4927-BC05-C3884855679C}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.6328125" customWidth="1"/>
-    <col min="2" max="2" width="11.08984375" style="13" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="13"/>
+    <col min="2" max="4" width="11.08984375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="14" style="9" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="12"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="15">
         <v>0.47799999999999998</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="15">
         <v>0.374</v>
       </c>
-      <c r="D3" s="17">
-        <f>AVERAGE(B3:C3)</f>
-        <v>0.42599999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D3" s="15">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="E3" s="15">
+        <v>0.439</v>
+      </c>
+      <c r="F3" s="16">
+        <f>AVERAGE(B3:E3)</f>
+        <v>0.42000000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="15">
         <v>0.35299999999999998</v>
       </c>
       <c r="C4" s="15">
         <v>0.27200000000000002</v>
       </c>
-      <c r="D4" s="24">
-        <f t="shared" ref="D4:D21" si="0">AVERAGE(B4:C4)</f>
-        <v>0.3125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D4" s="15">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0.318</v>
+      </c>
+      <c r="F4" s="10">
+        <f>AVERAGE(B4:E4)</f>
+        <v>0.30725000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="15">
         <v>0.60399999999999998</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="15">
         <v>0.54200000000000004</v>
       </c>
-      <c r="D5" s="18">
-        <f t="shared" si="0"/>
-        <v>0.57299999999999995</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D5" s="15">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="F5" s="17">
+        <f>AVERAGE(B5:E5)</f>
+        <v>0.56399999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="15">
         <v>0.47699999999999998</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="15">
         <v>0.376</v>
       </c>
-      <c r="D6" s="18">
-        <f t="shared" si="0"/>
-        <v>0.42649999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D6" s="15">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="F6" s="17">
+        <f>AVERAGE(B6:E6)</f>
+        <v>0.42600000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="15">
         <v>0.48499999999999999</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="15">
         <v>0.36499999999999999</v>
       </c>
-      <c r="D7" s="18">
-        <f t="shared" si="0"/>
-        <v>0.42499999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D7" s="15">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="F7" s="17">
+        <f>AVERAGE(B7:E7)</f>
+        <v>0.42574999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="15">
         <v>0.219</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="15">
         <v>0.21199999999999999</v>
       </c>
-      <c r="D8" s="22">
-        <f t="shared" si="0"/>
-        <v>0.2155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D8" s="15">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="F8" s="22">
+        <f>AVERAGE(B8:E8)</f>
+        <v>0.20900000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="15">
         <v>0.219</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="15">
         <v>0.21199999999999999</v>
       </c>
-      <c r="D9" s="22">
-        <f t="shared" si="0"/>
-        <v>0.2155</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D9" s="15">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="E9" s="15">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="F9" s="22">
+        <f>AVERAGE(B9:E9)</f>
+        <v>0.20900000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="15">
         <v>0.47699999999999998</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="15">
         <v>0.379</v>
       </c>
-      <c r="D10" s="18">
-        <f t="shared" si="0"/>
-        <v>0.42799999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D10" s="15">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="E10" s="15">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="F10" s="17">
+        <f>AVERAGE(B10:E10)</f>
+        <v>0.42374999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="15">
         <v>0.38400000000000001</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="15">
         <v>0.32100000000000001</v>
       </c>
-      <c r="D11" s="18">
-        <f t="shared" si="0"/>
-        <v>0.35250000000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D11" s="15">
+        <v>0.315</v>
+      </c>
+      <c r="E11" s="15">
+        <v>0.37</v>
+      </c>
+      <c r="F11" s="11">
+        <f>AVERAGE(B11:E11)</f>
+        <v>0.34750000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="15">
         <v>0.35299999999999998</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="15">
         <v>0.26900000000000002</v>
       </c>
-      <c r="D12" s="23">
-        <f t="shared" si="0"/>
-        <v>0.311</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D12" s="15">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="E12" s="15">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="F12" s="10">
+        <f>AVERAGE(B12:E12)</f>
+        <v>0.30674999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="15">
         <v>0.47599999999999998</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="15">
         <v>0.376</v>
       </c>
-      <c r="D13" s="18">
-        <f t="shared" si="0"/>
-        <v>0.42599999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D13" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="E13" s="15">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="F13" s="17">
+        <f>AVERAGE(B13:E13)</f>
+        <v>0.42649999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="15">
         <v>0.48</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="15">
         <v>0.38300000000000001</v>
       </c>
-      <c r="D14" s="18">
-        <f t="shared" si="0"/>
-        <v>0.43149999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D14" s="15">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="E14" s="15">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="F14" s="17">
+        <f>AVERAGE(B14:E14)</f>
+        <v>0.42675000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="15">
         <v>0.49</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="15">
         <v>0.42499999999999999</v>
       </c>
-      <c r="D15" s="18">
-        <f t="shared" si="0"/>
-        <v>0.45750000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D15" s="15">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="E15" s="15">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="F15" s="17">
+        <f>AVERAGE(B15:E15)</f>
+        <v>0.45800000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="15">
         <v>0.47699999999999998</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="15">
         <v>0.38300000000000001</v>
       </c>
-      <c r="D16" s="18">
-        <f t="shared" si="0"/>
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D16" s="15">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="E16" s="15">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="F16" s="17">
+        <f>AVERAGE(B16:E16)</f>
+        <v>0.42775000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="15">
         <v>0.51100000000000001</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="15">
         <v>0.45500000000000002</v>
       </c>
-      <c r="D17" s="18">
-        <f t="shared" si="0"/>
-        <v>0.48299999999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D17" s="15">
+        <v>0.443</v>
+      </c>
+      <c r="E17" s="15">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="F17" s="17">
+        <f>AVERAGE(B17:E17)</f>
+        <v>0.47950000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="15">
         <v>0.35799999999999998</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="15">
         <v>0.36799999999999999</v>
       </c>
-      <c r="D18" s="18">
-        <f t="shared" si="0"/>
-        <v>0.36299999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D18" s="15">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="E18" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="17">
+        <f>AVERAGE(B18:E18)</f>
+        <v>0.39224999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="15">
         <v>0.46200000000000002</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="15">
         <v>0.35899999999999999</v>
       </c>
-      <c r="D19" s="18">
-        <f t="shared" si="0"/>
-        <v>0.41049999999999998</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D19" s="15">
+        <v>0.35</v>
+      </c>
+      <c r="E19" s="15">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="F19" s="17">
+        <f>AVERAGE(B19:E19)</f>
+        <v>0.39224999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="15">
         <v>0.76200000000000001</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="15">
         <v>0.68600000000000005</v>
       </c>
-      <c r="D20" s="18">
-        <f t="shared" si="0"/>
-        <v>0.72399999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="8" t="s">
+      <c r="D20" s="15">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="E20" s="15">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="F20" s="17">
+        <f>AVERAGE(B20:E20)</f>
+        <v>0.67999999999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21" s="18">
         <v>0.17199999999999999</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="21">
         <v>0.19400000000000001</v>
       </c>
       <c r="D21" s="21">
-        <f t="shared" si="0"/>
-        <v>0.183</v>
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="E21" s="19">
+        <v>0.218</v>
+      </c>
+      <c r="F21" s="23">
+        <f>AVERAGE(B21:E21)</f>
+        <v>0.214</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>